<commit_message>
Cleaning up for demo2 work. Started demo 2 work.
</commit_message>
<xml_diff>
--- a/resources/Lake House Ref Architecture Specifications.xlsx
+++ b/resources/Lake House Ref Architecture Specifications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspaces\vr\repos\AWS-LakeHouse-Ref-Arch\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13479947-74E6-4582-92D7-4573C5840230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AB415B-2F00-41D0-811B-8D3EA15B1A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="0" windowWidth="26626" windowHeight="14685" xr2:uid="{C6B5E925-7FEF-4C0A-A848-7AE517B3EC43}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="16395" xr2:uid="{C6B5E925-7FEF-4C0A-A848-7AE517B3EC43}"/>
   </bookViews>
   <sheets>
     <sheet name="Permission Configs 1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>IAM</t>
   </si>
@@ -77,37 +77,6 @@
   </si>
   <si>
     <t>CF Template Resource Name Value</t>
-  </si>
-  <si>
-    <t>GlueStudioRole:
-    Type: 'AWS::IAM::Role'
-    Properties:
-      RoleName: !Sub "${Env}-lakehouse-${ComponentID}-glue-studio-role"
-      AssumeRolePolicyDocument:
-        Version: 2012-10-17
-        Statement:
-          - Effect: Allow
-            Principal:
-              Service: 'glue.amazonaws.com'
-            Action: 'sts:AssumeRole'
-      Path: /
-      ManagedPolicyArns:
-        - "arn:aws:iam::aws:policy/service-role/AWSGlueServiceRole"
-      Policies:
-        - PolicyName: !Sub "${Env}-${ComponentID}-lakehouse-role-policy"
-          PolicyDocument:
-            Version: 2012-10-17
-            Statement:
-              - Action:
-                  - "s3:*"
-                Effect: Allow
-                Resource: 
-                  - !Join [ '', ["arn:aws:s3:::", !Sub "${Env}", "-lakehouse-", !Sub "${ComponentID}", "-producer-bucket/*"]]
-                  - !Join [ '', ["arn:aws:s3:::", !Sub "${Env}", "-lakehouse-", !Sub "${ComponentID}", "-lz-bucket/*"]]
-                  - !Join [ '', ["arn:aws:s3:::", !Sub "${Env}", "-lakehouse-lh-s3-raw/*"]]
-                  - !Join [ '', ["arn:aws:s3:::", !Sub "${Env}", "-lakehouse-lh-s3-transformed/*"]]
-                  - !Join [ '', ["arn:aws:s3:::", !Sub "${Env}", "-lakehouse-lh-s3-curated/*"]]
-                  - !Join [ '', ["arn:aws:s3:::", !Sub "${Env}", "-lakehouse-lh-s3-glue-studio-temporary/*"]]</t>
   </si>
   <si>
     <t>RoleName: !Sub "${Env}-lakehouse-${ComponentID}-glue-studio-role"</t>
@@ -415,9 +384,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -435,6 +401,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,10 +419,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -756,10 +721,10 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -774,36 +739,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6"/>
+      <c r="G1" s="13"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="7" t="s">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -811,205 +776,203 @@
       <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="E4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" ht="204" x14ac:dyDescent="0.45">
-      <c r="A5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="9"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="9"/>
       <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="10"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="9"/>
       <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="10"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="9"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="9"/>
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="10"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="9"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="9"/>
       <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="9"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="9"/>
       <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="10"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="9"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="10"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="9"/>
       <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="10"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="9"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="10"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="9"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
@@ -1300,54 +1263,54 @@
         <v>8</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="313.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" s="2" t="s">
+      <c r="F12" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J11" s="2" t="s">
+      <c r="H12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
@@ -1360,6 +1323,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000D31F65C54552441B799AC8EB82A36AC" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fb172a2cd01a54621533907598ff36b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8cbf02a6-8340-459f-b54b-907f20541e8e" xmlns:ns4="4ddbdc53-0f8d-4edc-8cb6-c3e8a0a6859a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b6c14f1de3fd97364ba45f10db53e14" ns3:_="" ns4:_="">
     <xsd:import namespace="8cbf02a6-8340-459f-b54b-907f20541e8e"/>
@@ -1556,22 +1534,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0ADE7A4-F875-4B2D-9D26-8CBAE25CCAC5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="8cbf02a6-8340-459f-b54b-907f20541e8e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ddbdc53-0f8d-4edc-8cb6-c3e8a0a6859a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B77821F-F384-475D-8490-9A035A8FCDEC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B23DC64F-92E6-44B4-A488-5F7F6334C1CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1588,29 +1576,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0B77821F-F384-475D-8490-9A035A8FCDEC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C0ADE7A4-F875-4B2D-9D26-8CBAE25CCAC5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="8cbf02a6-8340-459f-b54b-907f20541e8e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ddbdc53-0f8d-4edc-8cb6-c3e8a0a6859a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>